<commit_message>
added modules: cwires, onfirst
</commit_message>
<xml_diff>
--- a/KeepTalking_Pins.xlsx
+++ b/KeepTalking_Pins.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dateien\Elektronik\Projekte\KeepTalkingBomb\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34776ADC-FBA3-43BF-BD6E-21E0F3935B32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9891ECDF-48FB-46A0-BBA8-00032302EA78}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{CEE79296-99E1-4E94-89D5-6769C9BCDA9F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="234">
   <si>
     <t>Pin</t>
   </si>
@@ -706,24 +706,9 @@
     <t>Button CodeOK</t>
   </si>
   <si>
-    <t>Button CodeCLR</t>
-  </si>
-  <si>
     <t>Morse</t>
   </si>
   <si>
-    <t>Code5</t>
-  </si>
-  <si>
-    <t>Code6</t>
-  </si>
-  <si>
-    <t>Button Timer1</t>
-  </si>
-  <si>
-    <t>Button Timer2</t>
-  </si>
-  <si>
     <t>LED Detonate</t>
   </si>
   <si>
@@ -731,6 +716,27 @@
   </si>
   <si>
     <t>LED Abort</t>
+  </si>
+  <si>
+    <t>Button Timer</t>
+  </si>
+  <si>
+    <t>LED Morse</t>
+  </si>
+  <si>
+    <t>CodeX1</t>
+  </si>
+  <si>
+    <t>CodeX2</t>
+  </si>
+  <si>
+    <t>CodeX3</t>
+  </si>
+  <si>
+    <t>Random seed</t>
+  </si>
+  <si>
+    <t>Vibrator</t>
   </si>
 </sst>
 </file>
@@ -1093,7 +1099,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0834993-2D73-4890-85C5-FC2C85A13B6A}">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1119,13 +1127,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>156</v>
-      </c>
-      <c r="D2">
-        <v>41</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1133,13 +1138,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D3">
-        <v>42</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1147,13 +1149,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>158</v>
-      </c>
-      <c r="D4">
-        <v>43</v>
+        <v>219</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1161,13 +1160,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>160</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D5">
-        <v>44</v>
+        <v>220</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1178,7 +1174,7 @@
         <v>73</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>221</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1186,10 +1182,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>155</v>
+        <v>73</v>
       </c>
       <c r="C7" t="s">
-        <v>229</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1197,10 +1193,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>155</v>
+        <v>223</v>
       </c>
       <c r="C8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1211,7 +1207,7 @@
         <v>155</v>
       </c>
       <c r="C9" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1219,10 +1215,10 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
       <c r="C10" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,10 +1226,10 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
       <c r="C11" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1241,10 +1237,13 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="C12" t="s">
-        <v>220</v>
+        <v>144</v>
+      </c>
+      <c r="D12">
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -1252,10 +1251,13 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
+        <v>143</v>
       </c>
       <c r="C13" t="s">
-        <v>221</v>
+        <v>145</v>
+      </c>
+      <c r="D13">
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1263,13 +1265,13 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>155</v>
+        <v>143</v>
       </c>
       <c r="C14" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D14">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -1280,10 +1282,10 @@
         <v>143</v>
       </c>
       <c r="C15" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D15">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1291,13 +1293,13 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="C16" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="D16">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1305,13 +1307,13 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>157</v>
       </c>
       <c r="D17">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1319,13 +1321,13 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="C18" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="D18">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1333,10 +1335,13 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>160</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>159</v>
+      </c>
+      <c r="D19">
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1399,13 +1404,10 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="C25" t="s">
-        <v>116</v>
-      </c>
-      <c r="D25">
-        <v>2</v>
+        <v>72</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1416,10 +1418,10 @@
         <v>75</v>
       </c>
       <c r="C26" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D26">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1430,10 +1432,10 @@
         <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D27">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1444,10 +1446,10 @@
         <v>75</v>
       </c>
       <c r="C28" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D28">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1458,10 +1460,10 @@
         <v>75</v>
       </c>
       <c r="C29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D29">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1472,10 +1474,10 @@
         <v>75</v>
       </c>
       <c r="C30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D30">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1486,10 +1488,10 @@
         <v>75</v>
       </c>
       <c r="C31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D31">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1500,10 +1502,10 @@
         <v>75</v>
       </c>
       <c r="C32" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D32">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1514,10 +1516,10 @@
         <v>75</v>
       </c>
       <c r="C33" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D33">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1528,10 +1530,10 @@
         <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="D34">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1542,10 +1544,10 @@
         <v>75</v>
       </c>
       <c r="C35" t="s">
-        <v>222</v>
+        <v>115</v>
       </c>
       <c r="D35">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1556,10 +1558,10 @@
         <v>75</v>
       </c>
       <c r="C36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D36">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1573,7 +1575,7 @@
         <v>126</v>
       </c>
       <c r="D37">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1587,7 +1589,7 @@
         <v>127</v>
       </c>
       <c r="D38">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1601,7 +1603,7 @@
         <v>128</v>
       </c>
       <c r="D39">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1615,7 +1617,7 @@
         <v>129</v>
       </c>
       <c r="D40">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1629,7 +1631,7 @@
         <v>130</v>
       </c>
       <c r="D41">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1643,7 +1645,7 @@
         <v>131</v>
       </c>
       <c r="D42">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1657,7 +1659,7 @@
         <v>132</v>
       </c>
       <c r="D43">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1671,7 +1673,7 @@
         <v>133</v>
       </c>
       <c r="D44">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1685,7 +1687,7 @@
         <v>134</v>
       </c>
       <c r="D45">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1699,7 +1701,7 @@
         <v>135</v>
       </c>
       <c r="D46">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1713,7 +1715,7 @@
         <v>142</v>
       </c>
       <c r="D47">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1738,7 +1740,7 @@
         <v>137</v>
       </c>
       <c r="D49">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1752,7 +1754,7 @@
         <v>138</v>
       </c>
       <c r="D50">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1766,7 +1768,7 @@
         <v>139</v>
       </c>
       <c r="D51">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1780,7 +1782,7 @@
         <v>140</v>
       </c>
       <c r="D52">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1794,7 +1796,7 @@
         <v>141</v>
       </c>
       <c r="D53">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1808,7 +1810,7 @@
         <v>197</v>
       </c>
       <c r="D54">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1822,7 +1824,7 @@
         <v>149</v>
       </c>
       <c r="D55">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1836,7 +1838,7 @@
         <v>150</v>
       </c>
       <c r="D56">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1850,7 +1852,7 @@
         <v>151</v>
       </c>
       <c r="D57">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1864,7 +1866,7 @@
         <v>152</v>
       </c>
       <c r="D58">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1878,7 +1880,7 @@
         <v>153</v>
       </c>
       <c r="D59">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1892,7 +1894,7 @@
         <v>154</v>
       </c>
       <c r="D60">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1914,10 +1916,10 @@
         <v>65</v>
       </c>
       <c r="B62" t="s">
-        <v>73</v>
+        <v>155</v>
       </c>
       <c r="C62" t="s">
-        <v>228</v>
+        <v>155</v>
       </c>
       <c r="D62">
         <v>1</v>
@@ -1926,6 +1928,12 @@
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>66</v>
+      </c>
+      <c r="B63" t="s">
+        <v>50</v>
+      </c>
+      <c r="C63" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -1940,7 +1948,7 @@
   <dimension ref="B2:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,7 +2092,7 @@
         <v>114</v>
       </c>
       <c r="J7" t="s">
-        <v>224</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
@@ -2105,7 +2113,7 @@
         <v>199</v>
       </c>
       <c r="J8" t="s">
-        <v>194</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
@@ -2120,13 +2128,13 @@
         <v>99</v>
       </c>
       <c r="H9" t="s">
-        <v>225</v>
+        <v>166</v>
       </c>
       <c r="I9" t="s">
-        <v>166</v>
+        <v>194</v>
       </c>
       <c r="J9" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
@@ -2141,10 +2149,10 @@
         <v>100</v>
       </c>
       <c r="H10" t="s">
-        <v>226</v>
+        <v>167</v>
       </c>
       <c r="I10" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="J10" t="s">
         <v>196</v>

</xml_diff>